<commit_message>
Update: tham gia PF từ một quốc gia khác
</commit_message>
<xml_diff>
--- a/Spotify/Code.xlsx
+++ b/Spotify/Code.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Freelance\Freelance_Project\Spotify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02C29815-B01B-407E-B214-CCEA7D67B0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34E8A44-AE41-4C04-90CB-73B6C6D2C7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{4074DFA8-510D-4E19-A697-E20CBF737DF8}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="12645" xr2:uid="{4074DFA8-510D-4E19-A697-E20CBF737DF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Message</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Thất bại, không thể thực hiện được</t>
+  </si>
+  <si>
+    <t>Tham gia Premium Family từ một quốc gia khác</t>
   </si>
 </sst>
 </file>
@@ -449,16 +452,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566D7DFF-18C9-42C6-9AFE-AA3C05626856}">
-  <dimension ref="B2:D10"/>
+  <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="C2:D10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="19.375" customWidth="1"/>
-    <col min="4" max="4" width="37" customWidth="1"/>
+    <col min="4" max="4" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
@@ -531,24 +534,33 @@
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="1">
+        <v>405</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="1">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
         <v>409</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>